<commit_message>
Dashboard Data extracted with UiPath
</commit_message>
<xml_diff>
--- a/Discovery Drive.xlsx
+++ b/Discovery Drive.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60eb891258ff8c93/Documents/PER - Personal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HobbyProjects\DriveAssistant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="965" documentId="14_{7B04147F-EF74-47FD-9932-EEE25F2E465B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6526EAF1-1889-4097-AA57-2B1193E6FC79}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B18F959C-2762-4863-8D45-CA77990E931F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
   </bookViews>
   <sheets>
     <sheet name="Discovery Drive" sheetId="2" r:id="rId1"/>
+    <sheet name="Drive" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
   <si>
     <t>End</t>
   </si>
@@ -111,6 +112,39 @@
   </si>
   <si>
     <t>Totals Drive Points</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Km/day</t>
+  </si>
+  <si>
+    <t>Points/day</t>
+  </si>
+  <si>
+    <t>Predict Status</t>
+  </si>
+  <si>
+    <t>Prediction</t>
+  </si>
+  <si>
+    <t>Ekstra</t>
+  </si>
+  <si>
+    <t>The predicted status gives a more realistic prediction of the driving status. If the rediction is disable, best case scenario is assumed, which is 50 point drive days and the distance remains in the same bracket.</t>
+  </si>
+  <si>
+    <t>Stefan</t>
+  </si>
+  <si>
+    <t>Average</t>
   </si>
 </sst>
 </file>
@@ -122,7 +156,7 @@
     <numFmt numFmtId="165" formatCode="[$R-1C09]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="[$R-1C09]#,##0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,8 +184,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,8 +211,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -214,12 +267,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -282,17 +355,67 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -312,14 +435,27 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/featurePropertyBag/featurePropertyBag.xml><?xml version="1.0" encoding="utf-8"?>
+<FeaturePropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag">
+  <bag type="Checkbox"/>
+  <bag type="XFControls">
+    <bagId k="CellControl">0</bagId>
+  </bag>
+  <bag type="XFComplement">
+    <bagId k="XFControls">1</bagId>
+  </bag>
+  <bag type="XFComplements" extRef="XFComplementsMapperExtRef">
+    <a k="MappedFeaturePropertyBags">
+      <bagId>2</bagId>
+    </a>
+  </bag>
+</FeaturePropertyBags>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -357,7 +493,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -463,7 +599,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -605,7 +741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -618,7 +754,9 @@
   </sheetPr>
   <dimension ref="B1:T45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:H30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -629,16 +767,28 @@
     <col min="5" max="5" width="8.88671875" style="6"/>
     <col min="6" max="6" width="11.109375" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="8.88671875" style="6"/>
-    <col min="9" max="9" width="2.6640625" style="6" hidden="1" customWidth="1"/>
-    <col min="10" max="12" width="8.88671875" style="6" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="2.6640625" style="6" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="17" hidden="1" customWidth="1"/>
-    <col min="15" max="17" width="8.88671875" style="6" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="2.6640625" style="6" customWidth="1"/>
+    <col min="10" max="12" width="8.88671875" style="6" customWidth="1"/>
+    <col min="13" max="13" width="2.6640625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="5" style="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.21875" style="6" bestFit="1" customWidth="1"/>
     <col min="18" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="N1" s="6"/>
+      <c r="J1" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="N1" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
     </row>
     <row r="2" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
@@ -646,7 +796,7 @@
       </c>
       <c r="C2" s="8">
         <f ca="1">IF(ROUND(DAY(EOMONTH(TODAY(),0))*AVERAGE(OFFSET(H2,0,0,COUNTA(H2:INDEX(H:H,DAY(EOMONTH(TODAY(),-1))+1)),1)),0)&gt;1500,1500,ROUND(DAY(EOMONTH(TODAY(),0))*AVERAGE(OFFSET(H2,0,0,COUNTA(H2:INDEX(H:H,DAY(EOMONTH(TODAY(),-1))+1)),1)),0))</f>
-        <v>1500</v>
+        <v>1476</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="7" t="s">
@@ -688,7 +838,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="1">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E3" s="10">
         <f ca="1">DATE(YEAR(TODAY()),MONTH(TODAY()),1)</f>
@@ -698,12 +848,11 @@
         <f ca="1">TEXT(E3,"dddd")</f>
         <v>Monday</v>
       </c>
-      <c r="G3" s="11">
-        <f>2.51+13.3+4.85+0.02+0.02+0.08+4.97+2.66+4.7+0.56+5.5+2.57</f>
-        <v>41.74</v>
+      <c r="G3" s="24">
+        <v>10.005000000000001</v>
       </c>
       <c r="H3" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J3" s="1">
         <v>0</v>
@@ -732,8 +881,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="1">
-        <f>300-5*2-33*2-5*2-10*4-10*2</f>
-        <v>154</v>
+        <v>300</v>
       </c>
       <c r="E4" s="10">
         <f ca="1">E3+1</f>
@@ -743,12 +891,11 @@
         <f t="shared" ref="F4:F30" ca="1" si="0">TEXT(E4,"dddd")</f>
         <v>Tuesday</v>
       </c>
-      <c r="G4" s="11">
-        <f>2.53+2.96+1.37+1.31+1.67</f>
-        <v>9.84</v>
+      <c r="G4" s="24">
+        <v>8.4209999999999994</v>
       </c>
       <c r="H4" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J4" s="1">
         <v>150</v>
@@ -778,7 +925,7 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">VLOOKUP(DAY(EOMONTH(TODAY(),0))*AVERAGE(OFFSET(G2,0,0,COUNTA(G2:INDEX(G:G,DAY(EOMONTH(TODAY(),-1))+1)),1)),J2:L17,3,TRUE)</f>
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="E5" s="10">
         <f t="shared" ref="E5:E33" ca="1" si="1">E4+1</f>
@@ -788,12 +935,11 @@
         <f t="shared" ca="1" si="0"/>
         <v>Wednesday</v>
       </c>
-      <c r="G5" s="11">
-        <f>1.98</f>
-        <v>1.98</v>
+      <c r="G5" s="24">
+        <v>21.553999999999998</v>
       </c>
       <c r="H5" s="1">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="J5" s="1">
         <v>300</v>
@@ -832,12 +978,11 @@
         <f t="shared" ca="1" si="0"/>
         <v>Thursday</v>
       </c>
-      <c r="G6" s="11">
-        <f>10.6+5.18+1.68</f>
-        <v>17.46</v>
+      <c r="G6" s="24">
+        <v>2.8559999999999999</v>
       </c>
       <c r="H6" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J6" s="1">
         <v>450</v>
@@ -867,7 +1012,7 @@
       </c>
       <c r="C7" s="8">
         <f ca="1">SUM(C2:C6)</f>
-        <v>2074</v>
+        <v>2476</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="10">
@@ -878,9 +1023,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>Friday</v>
       </c>
-      <c r="G7" s="11">
-        <f>1.7+2.37+2.5</f>
-        <v>6.57</v>
+      <c r="G7" s="24">
+        <v>69.301000000000002</v>
       </c>
       <c r="H7" s="1">
         <v>50</v>
@@ -916,9 +1060,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>Saturday</v>
       </c>
-      <c r="G8" s="11">
-        <f>2.55+1.62+4.24</f>
-        <v>8.41</v>
+      <c r="G8" s="24">
+        <v>103.66800000000001</v>
       </c>
       <c r="H8" s="1">
         <v>50</v>
@@ -940,7 +1083,7 @@
       </c>
       <c r="C9" s="1" t="str">
         <f ca="1">VLOOKUP(C7,N3:P7,3,TRUE)</f>
-        <v>Silver</v>
+        <v>Gold</v>
       </c>
       <c r="E9" s="10">
         <f t="shared" ca="1" si="1"/>
@@ -950,9 +1093,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="G9" s="11">
-        <f>2.57+21.69+22.93+2.55+2.58</f>
-        <v>52.319999999999993</v>
+      <c r="G9" s="24">
+        <v>103.31</v>
       </c>
       <c r="H9" s="1">
         <v>50</v>
@@ -990,9 +1132,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>Monday</v>
       </c>
-      <c r="G10" s="11">
-        <f>2.56+2.6+4.68+1+2.59</f>
-        <v>13.43</v>
+      <c r="G10" s="24">
+        <v>100.373</v>
       </c>
       <c r="H10" s="1">
         <v>50</v>
@@ -1029,9 +1170,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>Tuesday</v>
       </c>
-      <c r="G11" s="11">
-        <f>2.54+10.41+14.53+3.53+0.63+0.68+1.04+0.62+2.62</f>
-        <v>36.599999999999994</v>
+      <c r="G11" s="24">
+        <v>69.218999999999994</v>
       </c>
       <c r="H11" s="1">
         <v>50</v>
@@ -1060,9 +1200,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>Wednesday</v>
       </c>
-      <c r="G12" s="11">
-        <f>2.52+2.63+5.13</f>
-        <v>10.280000000000001</v>
+      <c r="G12" s="24">
+        <v>176.989</v>
       </c>
       <c r="H12" s="1">
         <v>50</v>
@@ -1092,9 +1231,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>Thursday</v>
       </c>
-      <c r="G13" s="11">
-        <f>2.58+12.71+0.39+5.8+7.81+4.64+11.24+2.43+2.48</f>
-        <v>50.08</v>
+      <c r="G13" s="24">
+        <v>69.213999999999999</v>
       </c>
       <c r="H13" s="1">
         <v>50</v>
@@ -1123,9 +1261,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>Friday</v>
       </c>
-      <c r="G14" s="11">
-        <f>5.11+1.11+4.93+11.14+4+5.17+11.51+5.01+3.56+1.41+10.36+11.19</f>
-        <v>74.5</v>
+      <c r="G14" s="24">
+        <v>107.149</v>
       </c>
       <c r="H14" s="1">
         <v>50</v>
@@ -1155,9 +1292,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>Saturday</v>
       </c>
-      <c r="G15" s="11">
-        <f>1.79+0.57+0.86+2.55+10.56+11.48</f>
-        <v>27.81</v>
+      <c r="G15" s="24">
+        <v>102.15</v>
       </c>
       <c r="H15" s="1">
         <v>50</v>
@@ -1186,9 +1322,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="G16" s="11">
-        <f>2.55+2.57</f>
-        <v>5.1199999999999992</v>
+      <c r="G16" s="24">
+        <v>69.168999999999997</v>
       </c>
       <c r="H16" s="1">
         <v>50</v>
@@ -1203,7 +1338,6 @@
         <v>40</v>
       </c>
       <c r="N16"/>
-      <c r="O16" s="23"/>
       <c r="P16"/>
       <c r="Q16"/>
       <c r="R16"/>
@@ -1218,9 +1352,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>Monday</v>
       </c>
-      <c r="G17" s="11">
-        <f>2.54+2.57</f>
-        <v>5.1099999999999994</v>
+      <c r="G17" s="24">
+        <v>68.802999999999997</v>
       </c>
       <c r="H17" s="1">
         <v>50</v>
@@ -1250,9 +1383,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>Tuesday</v>
       </c>
-      <c r="G18" s="11">
-        <f>1.05+2.03+1.04+12.6+0.03+3.76</f>
-        <v>20.509999999999998</v>
+      <c r="G18" s="24">
+        <v>69.105999999999995</v>
       </c>
       <c r="H18" s="1">
         <v>50</v>
@@ -1272,11 +1404,11 @@
         <f t="shared" ca="1" si="0"/>
         <v>Wednesday</v>
       </c>
-      <c r="G19" s="11">
-        <v>0</v>
+      <c r="G19" s="24">
+        <v>76.194000000000003</v>
       </c>
       <c r="H19" s="1">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N19"/>
       <c r="O19"/>
@@ -1293,9 +1425,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>Thursday</v>
       </c>
-      <c r="G20" s="11">
-        <f>2.56+6.7+32.26+17.62+1.11+8.87+22.02+7.19+1.01+2.58</f>
-        <v>101.92</v>
+      <c r="G20" s="24">
+        <v>64.850999999999999</v>
       </c>
       <c r="H20" s="1">
         <v>50</v>
@@ -1315,8 +1446,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>Friday</v>
       </c>
-      <c r="G21" s="11">
-        <v>2.44</v>
+      <c r="G21" s="24">
+        <v>49.548000000000002</v>
       </c>
       <c r="H21" s="1">
         <v>50</v>
@@ -1332,9 +1463,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>Saturday</v>
       </c>
-      <c r="G22" s="11">
-        <f>2.6+2.09+0.71+13.02+12.93+14.43+19.16+3.94+5.13</f>
-        <v>74.009999999999991</v>
+      <c r="G22" s="24">
+        <v>71.718999999999994</v>
       </c>
       <c r="H22" s="1">
         <v>50</v>
@@ -1351,9 +1481,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="G23" s="11">
-        <f>0.01+2.56+2.55+18.87+24.88+2.56</f>
-        <v>51.430000000000007</v>
+      <c r="G23" s="24">
+        <v>47.924999999999997</v>
       </c>
       <c r="H23" s="1">
         <v>50</v>
@@ -1371,9 +1500,8 @@
         <f t="shared" ca="1" si="0"/>
         <v>Monday</v>
       </c>
-      <c r="G24" s="11">
-        <f>18.06+17.19+2.54</f>
-        <v>37.79</v>
+      <c r="G24" s="24">
+        <v>31.699000000000002</v>
       </c>
       <c r="H24" s="1">
         <v>50</v>
@@ -1391,12 +1519,11 @@
         <f t="shared" ca="1" si="0"/>
         <v>Tuesday</v>
       </c>
-      <c r="G25" s="11">
-        <f>18.76+1.36+18.58+2.65+8.89+3.58+1.38+0.02+5.45</f>
-        <v>60.670000000000009</v>
+      <c r="G25" s="24">
+        <v>2.5960000000000001</v>
       </c>
       <c r="H25" s="1">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="N25" s="6"/>
       <c r="P25" s="2"/>
@@ -1410,11 +1537,12 @@
         <f t="shared" ca="1" si="0"/>
         <v>Wednesday</v>
       </c>
-      <c r="G26" s="11">
-        <f>34.86+31.92+8.95+2.6</f>
-        <v>78.33</v>
-      </c>
-      <c r="H26" s="1"/>
+      <c r="G26" s="24">
+        <v>37.198999999999998</v>
+      </c>
+      <c r="H26" s="1">
+        <v>50</v>
+      </c>
       <c r="N26" s="6"/>
       <c r="P26" s="2"/>
     </row>
@@ -1428,10 +1556,11 @@
         <v>Thursday</v>
       </c>
       <c r="G27" s="11">
-        <f>39.98+0.09+34.33+1.11+1.05+1.08+1.06</f>
-        <v>78.7</v>
-      </c>
-      <c r="H27" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
+        <v>50</v>
+      </c>
       <c r="N27" s="6"/>
       <c r="P27" s="2"/>
     </row>
@@ -1445,10 +1574,11 @@
         <v>Friday</v>
       </c>
       <c r="G28" s="11">
-        <f>34.89+0.08+51.98+0.01+2.3+46.85+55.21+78.71+8.24</f>
-        <v>278.27</v>
-      </c>
-      <c r="H28" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="1">
+        <v>50</v>
+      </c>
       <c r="N28" s="6"/>
       <c r="P28" s="2"/>
     </row>
@@ -1461,8 +1591,12 @@
         <f t="shared" ca="1" si="0"/>
         <v>Saturday</v>
       </c>
-      <c r="G29" s="11"/>
-      <c r="H29" s="1"/>
+      <c r="G29" s="11">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1">
+        <v>50</v>
+      </c>
       <c r="L29" s="3"/>
       <c r="N29" s="6"/>
     </row>
@@ -1475,11 +1609,15 @@
         <f t="shared" ca="1" si="0"/>
         <v>Sunday</v>
       </c>
-      <c r="G30" s="11"/>
-      <c r="H30" s="1"/>
+      <c r="G30" s="11">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1">
+        <v>50</v>
+      </c>
       <c r="N30" s="6"/>
     </row>
-    <row r="31" spans="2:18" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
       <c r="E31" s="10">
         <f t="shared" ca="1" si="1"/>
         <v>45502</v>
@@ -1488,8 +1626,13 @@
         <f t="shared" ref="F31:F33" ca="1" si="2">TEXT(E31,"dddd")</f>
         <v>Monday</v>
       </c>
-      <c r="G31" s="11"/>
-      <c r="H31" s="1"/>
+      <c r="G31" s="11">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0</v>
+      </c>
+      <c r="N31" s="6"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.3">
       <c r="E32" s="10">
@@ -1500,8 +1643,12 @@
         <f t="shared" ca="1" si="2"/>
         <v>Tuesday</v>
       </c>
-      <c r="G32" s="11"/>
-      <c r="H32" s="1"/>
+      <c r="G32" s="11">
+        <v>40</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0</v>
+      </c>
       <c r="N32" s="6"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.3">
@@ -1513,22 +1660,26 @@
         <f t="shared" ca="1" si="2"/>
         <v>Wednesday</v>
       </c>
-      <c r="G33" s="11"/>
-      <c r="H33" s="1"/>
+      <c r="G33" s="11">
+        <v>40</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0</v>
+      </c>
       <c r="N33" s="6"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="E34" s="24" t="s">
+      <c r="E34" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F34" s="25"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="18">
         <f>SUM(G3:G33)</f>
-        <v>1145.32</v>
+        <v>1613.018</v>
       </c>
       <c r="H34" s="8">
         <f>SUM(H3:H33)</f>
-        <v>1149</v>
+        <v>1381</v>
       </c>
       <c r="N34" s="6"/>
     </row>
@@ -1569,10 +1720,694 @@
       <c r="N45" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="N1:Q1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE70C601-B43B-41C4-8E7C-4A1600D76DAD}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:S50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" customWidth="1"/>
+    <col min="6" max="7" width="9.77734375" style="6" customWidth="1"/>
+    <col min="8" max="8" width="2.6640625" style="6" customWidth="1"/>
+    <col min="9" max="11" width="8.88671875" style="6" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="2.6640625" style="6" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="5" style="17" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="5" style="6" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="8.33203125" style="6" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="6.21875" style="6" hidden="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="39" t="str">
+        <f ca="1">_xlfn.CONCAT("Drive Summary ", M13, " ",TEXT(TODAY(), "mmmm yyyy"))</f>
+        <v>Drive Summary Stefan July 2024</v>
+      </c>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+    </row>
+    <row r="3" spans="2:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="28">
+        <f ca="1">IF(IF($C$16,G7,G6+G13)&gt;1500, 1500, IF($C$16,G7,G6+G13))</f>
+        <v>1500</v>
+      </c>
+      <c r="D5"/>
+      <c r="E5" s="7" t="str">
+        <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
+        <v>July 2024</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="41"/>
+      <c r="K5" s="23"/>
+      <c r="M5" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="26">
+        <v>300</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="34">
+        <v>1533.018</v>
+      </c>
+      <c r="G6" s="26">
+        <v>1381</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="26">
+        <v>300</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="28">
+        <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
+        <v>1697.2699285714286</v>
+      </c>
+      <c r="G7" s="28">
+        <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
+        <v>1528.9642857142856</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>149</v>
+      </c>
+      <c r="K7" s="1">
+        <v>300</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>799</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P7" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1">
+        <f>IF($C$16, VLOOKUP($F$7,$I$7:$K$21,3,TRUE),VLOOKUP($F$6,$I$7:$K$21,3,TRUE))</f>
+        <v>100</v>
+      </c>
+      <c r="F8" s="24"/>
+      <c r="G8" s="1"/>
+      <c r="I8" s="1">
+        <v>150</v>
+      </c>
+      <c r="J8" s="1">
+        <v>299</v>
+      </c>
+      <c r="K8" s="1">
+        <v>280</v>
+      </c>
+      <c r="M8" s="1">
+        <v>800</v>
+      </c>
+      <c r="N8" s="1">
+        <v>1599</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P8" s="12">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="26">
+        <v>300</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="1">
+        <v>300</v>
+      </c>
+      <c r="J9" s="1">
+        <v>449</v>
+      </c>
+      <c r="K9" s="1">
+        <v>260</v>
+      </c>
+      <c r="M9" s="1">
+        <v>1600</v>
+      </c>
+      <c r="N9" s="1">
+        <v>2199</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P9" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="R9" s="9"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="8">
+        <f ca="1">SUM(C5:C9)</f>
+        <v>2500</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="27">
+        <f ca="1">F6/(DAY(TODAY())-1)</f>
+        <v>54.750642857142857</v>
+      </c>
+      <c r="G10" s="27">
+        <f ca="1">G6/(DAY(TODAY())-1)</f>
+        <v>49.321428571428569</v>
+      </c>
+      <c r="I10" s="1">
+        <v>450</v>
+      </c>
+      <c r="J10" s="1">
+        <v>599</v>
+      </c>
+      <c r="K10" s="1">
+        <v>240</v>
+      </c>
+      <c r="M10" s="1">
+        <v>2200</v>
+      </c>
+      <c r="N10" s="1">
+        <v>2499</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P10" s="12">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="I11" s="1">
+        <v>600</v>
+      </c>
+      <c r="J11" s="1">
+        <v>749</v>
+      </c>
+      <c r="K11" s="1">
+        <v>220</v>
+      </c>
+      <c r="M11" s="5">
+        <v>2500</v>
+      </c>
+      <c r="N11" s="1">
+        <v>3000</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P11" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f ca="1">VLOOKUP(C10,M7:O11,3,TRUE)</f>
+        <v>Diamond</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="1">
+        <v>750</v>
+      </c>
+      <c r="J12" s="1">
+        <v>899</v>
+      </c>
+      <c r="K12" s="1">
+        <v>200</v>
+      </c>
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="13">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="38">
+        <f>VLOOKUP(F6,I7:K21,2,TRUE)-F6</f>
+        <v>115.98199999999997</v>
+      </c>
+      <c r="G13" s="33">
+        <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
+        <v>150</v>
+      </c>
+      <c r="I13" s="1">
+        <v>900</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1049</v>
+      </c>
+      <c r="K13" s="1">
+        <v>180</v>
+      </c>
+      <c r="M13" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="N13" s="42"/>
+      <c r="O13"/>
+      <c r="P13"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="15">
+        <f ca="1">C13*VLOOKUP(C12,O6:P11,2,FALSE)*10</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1050</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1199</v>
+      </c>
+      <c r="K14" s="1">
+        <v>160</v>
+      </c>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="S14" s="2"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="D15" s="14"/>
+      <c r="I15" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1349</v>
+      </c>
+      <c r="K15" s="1">
+        <v>140</v>
+      </c>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B16" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1350</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1499</v>
+      </c>
+      <c r="K16" s="1">
+        <v>120</v>
+      </c>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+    </row>
+    <row r="17" spans="2:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="I17" s="1">
+        <v>1500</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1649</v>
+      </c>
+      <c r="K17" s="1">
+        <v>100</v>
+      </c>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="I18" s="1">
+        <v>1650</v>
+      </c>
+      <c r="J18" s="1">
+        <v>1799</v>
+      </c>
+      <c r="K18" s="1">
+        <v>80</v>
+      </c>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="I19" s="1">
+        <v>1800</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1949</v>
+      </c>
+      <c r="K19" s="1">
+        <v>60</v>
+      </c>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="I20" s="1">
+        <v>1950</v>
+      </c>
+      <c r="J20" s="1">
+        <v>2099</v>
+      </c>
+      <c r="K20" s="1">
+        <v>40</v>
+      </c>
+      <c r="M20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="I21" s="1">
+        <v>2100</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
+        <v>20</v>
+      </c>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="Q22"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B23" s="3"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24" s="21"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25" s="21"/>
+      <c r="P25"/>
+      <c r="Q25"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="O26" s="2"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M27" s="6"/>
+      <c r="O27" s="2"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M28" s="6"/>
+      <c r="O28" s="2"/>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B29" s="2"/>
+      <c r="J29" s="4"/>
+      <c r="M29" s="6"/>
+      <c r="O29" s="2"/>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M30" s="6"/>
+      <c r="O30" s="2"/>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="30"/>
+      <c r="M31" s="6"/>
+      <c r="O31" s="2"/>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="E32" s="29"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="30"/>
+      <c r="M32" s="6"/>
+      <c r="O32" s="2"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="E33" s="29"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="30"/>
+      <c r="M33" s="6"/>
+      <c r="O33" s="2"/>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="E34" s="29"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="30"/>
+      <c r="K34" s="3"/>
+      <c r="M34" s="6"/>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="E35" s="29"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="30"/>
+      <c r="M35" s="6"/>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="E36" s="29"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="30"/>
+      <c r="M36" s="6"/>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="E37" s="29"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="30"/>
+      <c r="M37" s="6"/>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="E38" s="29"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="30"/>
+      <c r="M38" s="6"/>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="E39" s="29"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="32"/>
+      <c r="M39" s="6"/>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="H41" s="19"/>
+      <c r="M41" s="6"/>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B42" s="19"/>
+      <c r="M42" s="6"/>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M43" s="6"/>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="I44" s="3"/>
+      <c r="M44" s="6"/>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M45" s="6"/>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M46" s="6"/>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M47" s="6"/>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M48" s="6"/>
+    </row>
+    <row r="49" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M49" s="6"/>
+    </row>
+    <row r="50" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M50" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="M5:P5"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="B2:G3"/>
+    <mergeCell ref="B17:G19"/>
+    <mergeCell ref="I5:K5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Works for S and C on old DQMapper
</commit_message>
<xml_diff>
--- a/Discovery Drive.xlsx
+++ b/Discovery Drive.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HobbyProjects\DriveAssistant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\StefanOberholzer\GitGud\DriveAssistant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B18F959C-2762-4863-8D45-CA77990E931F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFCCA88-6ACB-4BFA-BED9-017C3AB0E509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
   </bookViews>
   <sheets>
     <sheet name="Discovery Drive" sheetId="2" r:id="rId1"/>
@@ -292,7 +292,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -355,16 +355,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -374,17 +365,14 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -401,21 +389,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -758,45 +751,45 @@
       <selection activeCell="E2" sqref="E2:H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.6640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="6"/>
-    <col min="6" max="6" width="11.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.88671875" style="6"/>
-    <col min="9" max="9" width="2.6640625" style="6" customWidth="1"/>
-    <col min="10" max="12" width="8.88671875" style="6" customWidth="1"/>
-    <col min="13" max="13" width="2.6640625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="6"/>
+    <col min="6" max="6" width="11.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="9" width="2.7109375" style="6" customWidth="1"/>
+    <col min="10" max="12" width="8.85546875" style="6" customWidth="1"/>
+    <col min="13" max="13" width="2.7109375" style="6" customWidth="1"/>
     <col min="14" max="14" width="5" style="17" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.21875" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.88671875" style="6"/>
+    <col min="16" max="16" width="8.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="J1" s="25" t="s">
+    <row r="1" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="J1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="N1" s="25" t="s">
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="N1" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-    </row>
-    <row r="2" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+    </row>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="8">
         <f ca="1">IF(ROUND(DAY(EOMONTH(TODAY(),0))*AVERAGE(OFFSET(H2,0,0,COUNTA(H2:INDEX(H:H,DAY(EOMONTH(TODAY(),-1))+1)),1)),0)&gt;1500,1500,ROUND(DAY(EOMONTH(TODAY(),0))*AVERAGE(OFFSET(H2,0,0,COUNTA(H2:INDEX(H:H,DAY(EOMONTH(TODAY(),-1))+1)),1)),0))</f>
-        <v>1476</v>
+        <v>1427</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="7" t="s">
@@ -833,7 +826,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
@@ -842,13 +835,13 @@
       </c>
       <c r="E3" s="10">
         <f ca="1">DATE(YEAR(TODAY()),MONTH(TODAY()),1)</f>
-        <v>45474</v>
+        <v>45505</v>
       </c>
       <c r="F3" s="1" t="str">
         <f ca="1">TEXT(E3,"dddd")</f>
-        <v>Monday</v>
-      </c>
-      <c r="G3" s="24">
+        <v>Thursday</v>
+      </c>
+      <c r="G3" s="22">
         <v>10.005000000000001</v>
       </c>
       <c r="H3" s="1">
@@ -876,7 +869,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
@@ -885,13 +878,13 @@
       </c>
       <c r="E4" s="10">
         <f ca="1">E3+1</f>
-        <v>45475</v>
+        <v>45506</v>
       </c>
       <c r="F4" s="1" t="str">
         <f t="shared" ref="F4:F30" ca="1" si="0">TEXT(E4,"dddd")</f>
-        <v>Tuesday</v>
-      </c>
-      <c r="G4" s="24">
+        <v>Friday</v>
+      </c>
+      <c r="G4" s="22">
         <v>8.4209999999999994</v>
       </c>
       <c r="H4" s="1">
@@ -919,7 +912,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
@@ -929,13 +922,13 @@
       </c>
       <c r="E5" s="10">
         <f t="shared" ref="E5:E33" ca="1" si="1">E4+1</f>
-        <v>45476</v>
+        <v>45507</v>
       </c>
       <c r="F5" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Wednesday</v>
-      </c>
-      <c r="G5" s="24">
+        <v>Saturday</v>
+      </c>
+      <c r="G5" s="22">
         <v>21.553999999999998</v>
       </c>
       <c r="H5" s="1">
@@ -963,7 +956,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
@@ -972,13 +965,13 @@
       </c>
       <c r="E6" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45477</v>
+        <v>45508</v>
       </c>
       <c r="F6" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Thursday</v>
-      </c>
-      <c r="G6" s="24">
+        <v>Sunday</v>
+      </c>
+      <c r="G6" s="22">
         <v>2.8559999999999999</v>
       </c>
       <c r="H6" s="1">
@@ -1006,24 +999,24 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="8">
         <f ca="1">SUM(C2:C6)</f>
-        <v>2476</v>
+        <v>2427</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45478</v>
+        <v>45509</v>
       </c>
       <c r="F7" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Friday</v>
-      </c>
-      <c r="G7" s="24">
+        <v>Monday</v>
+      </c>
+      <c r="G7" s="22">
         <v>69.301000000000002</v>
       </c>
       <c r="H7" s="1">
@@ -1051,16 +1044,16 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E8" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45479</v>
+        <v>45510</v>
       </c>
       <c r="F8" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Saturday</v>
-      </c>
-      <c r="G8" s="24">
+        <v>Tuesday</v>
+      </c>
+      <c r="G8" s="22">
         <v>103.66800000000001</v>
       </c>
       <c r="H8" s="1">
@@ -1077,7 +1070,7 @@
       </c>
       <c r="N8" s="6"/>
     </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
@@ -1087,13 +1080,13 @@
       </c>
       <c r="E9" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45480</v>
+        <v>45511</v>
       </c>
       <c r="F9" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Sunday</v>
-      </c>
-      <c r="G9" s="24">
+        <v>Wednesday</v>
+      </c>
+      <c r="G9" s="22">
         <v>103.31</v>
       </c>
       <c r="H9" s="1">
@@ -1115,7 +1108,7 @@
       <c r="R9"/>
       <c r="T9" s="2"/>
     </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>2</v>
       </c>
@@ -1126,13 +1119,13 @@
       <c r="D10" s="14"/>
       <c r="E10" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45481</v>
+        <v>45512</v>
       </c>
       <c r="F10" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Monday</v>
-      </c>
-      <c r="G10" s="24">
+        <v>Thursday</v>
+      </c>
+      <c r="G10" s="22">
         <v>100.373</v>
       </c>
       <c r="H10" s="1">
@@ -1153,7 +1146,7 @@
       <c r="Q10"/>
       <c r="R10"/>
     </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>1</v>
       </c>
@@ -1164,13 +1157,13 @@
       <c r="D11" s="16"/>
       <c r="E11" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45482</v>
+        <v>45513</v>
       </c>
       <c r="F11" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Tuesday</v>
-      </c>
-      <c r="G11" s="24">
+        <v>Friday</v>
+      </c>
+      <c r="G11" s="22">
         <v>69.218999999999994</v>
       </c>
       <c r="H11" s="1">
@@ -1191,16 +1184,16 @@
       <c r="Q11"/>
       <c r="R11"/>
     </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E12" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45483</v>
+        <v>45514</v>
       </c>
       <c r="F12" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Wednesday</v>
-      </c>
-      <c r="G12" s="24">
+        <v>Saturday</v>
+      </c>
+      <c r="G12" s="22">
         <v>176.989</v>
       </c>
       <c r="H12" s="1">
@@ -1221,17 +1214,17 @@
       <c r="Q12"/>
       <c r="R12"/>
     </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C13" s="20"/>
       <c r="E13" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45484</v>
+        <v>45515</v>
       </c>
       <c r="F13" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Thursday</v>
-      </c>
-      <c r="G13" s="24">
+        <v>Sunday</v>
+      </c>
+      <c r="G13" s="22">
         <v>69.213999999999999</v>
       </c>
       <c r="H13" s="1">
@@ -1252,16 +1245,16 @@
       <c r="Q13"/>
       <c r="R13"/>
     </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E14" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45485</v>
+        <v>45516</v>
       </c>
       <c r="F14" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Friday</v>
-      </c>
-      <c r="G14" s="24">
+        <v>Monday</v>
+      </c>
+      <c r="G14" s="22">
         <v>107.149</v>
       </c>
       <c r="H14" s="1">
@@ -1282,17 +1275,17 @@
       <c r="Q14"/>
       <c r="R14"/>
     </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C15" s="14"/>
       <c r="E15" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45486</v>
+        <v>45517</v>
       </c>
       <c r="F15" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Saturday</v>
-      </c>
-      <c r="G15" s="24">
+        <v>Tuesday</v>
+      </c>
+      <c r="G15" s="22">
         <v>102.15</v>
       </c>
       <c r="H15" s="1">
@@ -1313,16 +1306,16 @@
       <c r="Q15"/>
       <c r="R15"/>
     </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E16" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45487</v>
+        <v>45518</v>
       </c>
       <c r="F16" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Sunday</v>
-      </c>
-      <c r="G16" s="24">
+        <v>Wednesday</v>
+      </c>
+      <c r="G16" s="22">
         <v>69.168999999999997</v>
       </c>
       <c r="H16" s="1">
@@ -1342,17 +1335,17 @@
       <c r="Q16"/>
       <c r="R16"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C17" s="3"/>
       <c r="E17" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45488</v>
+        <v>45519</v>
       </c>
       <c r="F17" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Monday</v>
-      </c>
-      <c r="G17" s="24">
+        <v>Thursday</v>
+      </c>
+      <c r="G17" s="22">
         <v>68.802999999999997</v>
       </c>
       <c r="H17" s="1">
@@ -1373,17 +1366,17 @@
       <c r="Q17"/>
       <c r="R17"/>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="E18" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45489</v>
+        <v>45520</v>
       </c>
       <c r="F18" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Tuesday</v>
-      </c>
-      <c r="G18" s="24">
+        <v>Friday</v>
+      </c>
+      <c r="G18" s="22">
         <v>69.105999999999995</v>
       </c>
       <c r="H18" s="1">
@@ -1395,16 +1388,16 @@
       <c r="Q18"/>
       <c r="R18"/>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E19" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45490</v>
+        <v>45521</v>
       </c>
       <c r="F19" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Wednesday</v>
-      </c>
-      <c r="G19" s="24">
+        <v>Saturday</v>
+      </c>
+      <c r="G19" s="22">
         <v>76.194000000000003</v>
       </c>
       <c r="H19" s="1">
@@ -1416,16 +1409,16 @@
       <c r="Q19"/>
       <c r="R19"/>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E20" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45491</v>
+        <v>45522</v>
       </c>
       <c r="F20" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Thursday</v>
-      </c>
-      <c r="G20" s="24">
+        <v>Sunday</v>
+      </c>
+      <c r="G20" s="22">
         <v>64.850999999999999</v>
       </c>
       <c r="H20" s="1">
@@ -1437,16 +1430,16 @@
       <c r="Q20"/>
       <c r="R20"/>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E21" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45492</v>
+        <v>45523</v>
       </c>
       <c r="F21" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Friday</v>
-      </c>
-      <c r="G21" s="24">
+        <v>Monday</v>
+      </c>
+      <c r="G21" s="22">
         <v>49.548000000000002</v>
       </c>
       <c r="H21" s="1">
@@ -1454,16 +1447,16 @@
       </c>
       <c r="P21" s="2"/>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E22" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45493</v>
+        <v>45524</v>
       </c>
       <c r="F22" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Saturday</v>
-      </c>
-      <c r="G22" s="24">
+        <v>Tuesday</v>
+      </c>
+      <c r="G22" s="22">
         <v>71.718999999999994</v>
       </c>
       <c r="H22" s="1">
@@ -1472,16 +1465,16 @@
       <c r="N22" s="6"/>
       <c r="P22" s="2"/>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E23" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45494</v>
+        <v>45525</v>
       </c>
       <c r="F23" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Sunday</v>
-      </c>
-      <c r="G23" s="24">
+        <v>Wednesday</v>
+      </c>
+      <c r="G23" s="22">
         <v>47.924999999999997</v>
       </c>
       <c r="H23" s="1">
@@ -1490,17 +1483,17 @@
       <c r="N23" s="6"/>
       <c r="P23" s="2"/>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="E24" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45495</v>
+        <v>45526</v>
       </c>
       <c r="F24" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Monday</v>
-      </c>
-      <c r="G24" s="24">
+        <v>Thursday</v>
+      </c>
+      <c r="G24" s="22">
         <v>31.699000000000002</v>
       </c>
       <c r="H24" s="1">
@@ -1510,16 +1503,16 @@
       <c r="N24" s="6"/>
       <c r="P24" s="2"/>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E25" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45496</v>
+        <v>45527</v>
       </c>
       <c r="F25" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Tuesday</v>
-      </c>
-      <c r="G25" s="24">
+        <v>Friday</v>
+      </c>
+      <c r="G25" s="22">
         <v>2.5960000000000001</v>
       </c>
       <c r="H25" s="1">
@@ -1528,16 +1521,16 @@
       <c r="N25" s="6"/>
       <c r="P25" s="2"/>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E26" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45497</v>
+        <v>45528</v>
       </c>
       <c r="F26" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Wednesday</v>
-      </c>
-      <c r="G26" s="24">
+        <v>Saturday</v>
+      </c>
+      <c r="G26" s="22">
         <v>37.198999999999998</v>
       </c>
       <c r="H26" s="1">
@@ -1546,14 +1539,14 @@
       <c r="N26" s="6"/>
       <c r="P26" s="2"/>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E27" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45498</v>
+        <v>45529</v>
       </c>
       <c r="F27" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Thursday</v>
+        <v>Sunday</v>
       </c>
       <c r="G27" s="11">
         <v>0</v>
@@ -1564,14 +1557,14 @@
       <c r="N27" s="6"/>
       <c r="P27" s="2"/>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E28" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45499</v>
+        <v>45530</v>
       </c>
       <c r="F28" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Friday</v>
+        <v>Monday</v>
       </c>
       <c r="G28" s="11">
         <v>0</v>
@@ -1582,14 +1575,14 @@
       <c r="N28" s="6"/>
       <c r="P28" s="2"/>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E29" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45500</v>
+        <v>45531</v>
       </c>
       <c r="F29" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Saturday</v>
+        <v>Tuesday</v>
       </c>
       <c r="G29" s="11">
         <v>0</v>
@@ -1600,14 +1593,14 @@
       <c r="L29" s="3"/>
       <c r="N29" s="6"/>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E30" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45501</v>
+        <v>45532</v>
       </c>
       <c r="F30" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Sunday</v>
+        <v>Wednesday</v>
       </c>
       <c r="G30" s="11">
         <v>0</v>
@@ -1617,14 +1610,14 @@
       </c>
       <c r="N30" s="6"/>
     </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E31" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45502</v>
+        <v>45533</v>
       </c>
       <c r="F31" s="1" t="str">
         <f t="shared" ref="F31:F33" ca="1" si="2">TEXT(E31,"dddd")</f>
-        <v>Monday</v>
+        <v>Thursday</v>
       </c>
       <c r="G31" s="11">
         <v>0</v>
@@ -1634,14 +1627,14 @@
       </c>
       <c r="N31" s="6"/>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E32" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45503</v>
+        <v>45534</v>
       </c>
       <c r="F32" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Tuesday</v>
+        <v>Friday</v>
       </c>
       <c r="G32" s="11">
         <v>40</v>
@@ -1651,14 +1644,14 @@
       </c>
       <c r="N32" s="6"/>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E33" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45504</v>
+        <v>45535</v>
       </c>
       <c r="F33" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Wednesday</v>
+        <v>Saturday</v>
       </c>
       <c r="G33" s="11">
         <v>40</v>
@@ -1668,11 +1661,11 @@
       </c>
       <c r="N33" s="6"/>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="E34" s="22" t="s">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E34" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="18">
         <f>SUM(G3:G33)</f>
         <v>1613.018</v>
@@ -1683,40 +1676,40 @@
       </c>
       <c r="N34" s="6"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I36" s="19"/>
       <c r="N36" s="6"/>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" s="19"/>
       <c r="N37" s="6"/>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N38" s="6"/>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="J39" s="3"/>
       <c r="N39" s="6"/>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N40" s="6"/>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N41" s="6"/>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N42" s="6"/>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N43" s="6"/>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N44" s="6"/>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N45" s="6"/>
     </row>
   </sheetData>
@@ -1742,55 +1735,55 @@
       <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.6640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" customWidth="1"/>
-    <col min="6" max="7" width="9.77734375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="2.6640625" style="6" customWidth="1"/>
-    <col min="9" max="11" width="8.88671875" style="6" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="2.6640625" style="6" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="6" max="7" width="9.7109375" style="6" customWidth="1"/>
+    <col min="8" max="8" width="2.7109375" style="6" customWidth="1"/>
+    <col min="9" max="11" width="8.85546875" style="6" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="2.7109375" style="6" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="5" style="17" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="5" style="6" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="8.33203125" style="6" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="6.21875" style="6" hidden="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.88671875" style="6"/>
+    <col min="15" max="15" width="8.28515625" style="6" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="6.28515625" style="6" hidden="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="39" t="str">
+    <row r="2" spans="2:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="38" t="str">
         <f ca="1">_xlfn.CONCAT("Drive Summary ", M13, " ",TEXT(TODAY(), "mmmm yyyy"))</f>
-        <v>Drive Summary Stefan July 2024</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-    </row>
-    <row r="3" spans="2:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-    </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
+        <v>Drive Summary Stefan August 2024</v>
+      </c>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+    </row>
+    <row r="3" spans="2:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="25">
         <f ca="1">IF(IF($C$16,G7,G6+G13)&gt;1500, 1500, IF($C$16,G7,G6+G13))</f>
         <v>1500</v>
       </c>
       <c r="D5"/>
       <c r="E5" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
-        <v>July 2024</v>
+        <v>August 2024</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>20</v>
@@ -1798,32 +1791,32 @@
       <c r="G5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="41"/>
-      <c r="K5" s="23"/>
-      <c r="M5" s="22" t="s">
+      <c r="J5" s="36"/>
+      <c r="K5" s="34"/>
+      <c r="M5" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="N5" s="41"/>
-      <c r="O5" s="41"/>
-      <c r="P5" s="41"/>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="N5" s="36"/>
+      <c r="O5" s="36"/>
+      <c r="P5" s="36"/>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="23">
         <v>300</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="34">
+      <c r="F6" s="30">
         <v>1533.018</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="23">
         <v>1381</v>
       </c>
       <c r="I6" s="7" t="s">
@@ -1848,24 +1841,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="23">
         <v>300</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="25">
         <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>1697.2699285714286</v>
-      </c>
-      <c r="G7" s="28">
+        <v>6789.0797142857145</v>
+      </c>
+      <c r="G7" s="25">
         <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>1528.9642857142856</v>
+        <v>6115.8571428571422</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
@@ -1889,7 +1882,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1897,7 +1890,7 @@
         <f>IF($C$16, VLOOKUP($F$7,$I$7:$K$21,3,TRUE),VLOOKUP($F$6,$I$7:$K$21,3,TRUE))</f>
         <v>100</v>
       </c>
-      <c r="F8" s="24"/>
+      <c r="F8" s="22"/>
       <c r="G8" s="1"/>
       <c r="I8" s="1">
         <v>150</v>
@@ -1921,11 +1914,11 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="23">
         <v>300</v>
       </c>
       <c r="E9" s="7" t="s">
@@ -1960,7 +1953,7 @@
       </c>
       <c r="R9" s="9"/>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>5</v>
       </c>
@@ -1971,13 +1964,13 @@
       <c r="E10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="24">
         <f ca="1">F6/(DAY(TODAY())-1)</f>
-        <v>54.750642857142857</v>
-      </c>
-      <c r="G10" s="27">
+        <v>219.00257142857143</v>
+      </c>
+      <c r="G10" s="24">
         <f ca="1">G6/(DAY(TODAY())-1)</f>
-        <v>49.321428571428569</v>
+        <v>197.28571428571428</v>
       </c>
       <c r="I10" s="1">
         <v>450</v>
@@ -2001,7 +1994,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="I11" s="1">
         <v>600</v>
       </c>
@@ -2024,7 +2017,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
@@ -2033,7 +2026,7 @@
         <v>Diamond</v>
       </c>
       <c r="D12" s="9"/>
-      <c r="E12" s="29"/>
+      <c r="E12" s="26"/>
       <c r="F12" s="7" t="s">
         <v>20</v>
       </c>
@@ -2051,7 +2044,7 @@
       </c>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
@@ -2062,13 +2055,13 @@
       <c r="E13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="38">
+      <c r="F13" s="25">
         <f>VLOOKUP(F6,I7:K21,2,TRUE)-F6</f>
         <v>115.98199999999997</v>
       </c>
-      <c r="G13" s="33">
+      <c r="G13" s="1">
         <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
-        <v>150</v>
+        <v>1200</v>
       </c>
       <c r="I13" s="1">
         <v>900</v>
@@ -2079,14 +2072,14 @@
       <c r="K13" s="1">
         <v>180</v>
       </c>
-      <c r="M13" s="42" t="s">
+      <c r="M13" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="N13" s="42"/>
+      <c r="N13" s="37"/>
       <c r="O13"/>
       <c r="P13"/>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>1</v>
       </c>
@@ -2110,7 +2103,7 @@
       <c r="Q14"/>
       <c r="S14" s="2"/>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D15" s="14"/>
       <c r="I15" s="1">
         <v>1200</v>
@@ -2127,11 +2120,11 @@
       <c r="P15"/>
       <c r="Q15"/>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B16" s="40" t="s">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="35" t="b">
+      <c r="C16" s="31" t="b">
         <v>0</v>
       </c>
       <c r="I16" s="1">
@@ -2149,15 +2142,15 @@
       <c r="P16"/>
       <c r="Q16"/>
     </row>
-    <row r="17" spans="2:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="36" t="s">
+    <row r="17" spans="2:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
       <c r="I17" s="1">
         <v>1500</v>
       </c>
@@ -2173,13 +2166,13 @@
       <c r="P17"/>
       <c r="Q17"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
       <c r="I18" s="1">
         <v>1650</v>
       </c>
@@ -2195,13 +2188,13 @@
       <c r="P18"/>
       <c r="Q18"/>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
       <c r="I19" s="1">
         <v>1800</v>
       </c>
@@ -2217,13 +2210,13 @@
       <c r="P19"/>
       <c r="Q19"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
       <c r="I20" s="1">
         <v>1950</v>
       </c>
@@ -2238,10 +2231,10 @@
       <c r="P20"/>
       <c r="Q20"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
       <c r="I21" s="1">
         <v>2100</v>
       </c>
@@ -2257,13 +2250,13 @@
       <c r="P21"/>
       <c r="Q21"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
       <c r="Q22"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="M23"/>
       <c r="N23"/>
@@ -2271,133 +2264,133 @@
       <c r="P23"/>
       <c r="Q23"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M24"/>
       <c r="N24"/>
       <c r="O24" s="21"/>
       <c r="P24"/>
       <c r="Q24"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M25"/>
       <c r="N25"/>
       <c r="O25" s="21"/>
       <c r="P25"/>
       <c r="Q25"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="O26" s="2"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M27" s="6"/>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M28" s="6"/>
       <c r="O28" s="2"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="J29" s="4"/>
       <c r="M29" s="6"/>
       <c r="O29" s="2"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="M30" s="6"/>
       <c r="O30" s="2"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="30"/>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="27"/>
       <c r="M31" s="6"/>
       <c r="O31" s="2"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="E32" s="29"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="30"/>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="E32" s="26"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="27"/>
       <c r="M32" s="6"/>
       <c r="O32" s="2"/>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="E33" s="29"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="30"/>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E33" s="26"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="27"/>
       <c r="M33" s="6"/>
       <c r="O33" s="2"/>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="E34" s="29"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="30"/>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E34" s="26"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="27"/>
       <c r="K34" s="3"/>
       <c r="M34" s="6"/>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="E35" s="29"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="30"/>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E35" s="26"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="27"/>
       <c r="M35" s="6"/>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="E36" s="29"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="30"/>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E36" s="26"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="27"/>
       <c r="M36" s="6"/>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="E37" s="29"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="30"/>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E37" s="26"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="27"/>
       <c r="M37" s="6"/>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="E38" s="29"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="30"/>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E38" s="26"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="27"/>
       <c r="M38" s="6"/>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="E39" s="29"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="32"/>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E39" s="26"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="29"/>
       <c r="M39" s="6"/>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H41" s="19"/>
       <c r="M41" s="6"/>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42" s="19"/>
       <c r="M42" s="6"/>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M43" s="6"/>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I44" s="3"/>
       <c r="M44" s="6"/>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M45" s="6"/>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M46" s="6"/>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M47" s="6"/>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M48" s="6"/>
     </row>
-    <row r="49" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M49" s="6"/>
     </row>
-    <row r="50" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M50" s="6"/>
     </row>
   </sheetData>

</xml_diff>